<commit_message>
The register is now work
</commit_message>
<xml_diff>
--- a/Estoque e registro.xlsx
+++ b/Estoque e registro.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="15600" windowHeight="19440" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estoque" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Registro" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -208,52 +208,44 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" pivotButton="0" quotePrefix="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" pivotButton="0" quotePrefix="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
-    <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="3" builtinId="32"/>
+    <cellStyle name="Ênfase1" xfId="1" builtinId="29"/>
+    <cellStyle name="40% - Ênfase1" xfId="2" builtinId="31"/>
+    <cellStyle name="60% - Ênfase1" xfId="3" builtinId="32"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -656,25 +648,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="17.85546875" customWidth="1" style="21" min="1" max="1"/>
-    <col width="9.140625" customWidth="1" style="21" min="4" max="4"/>
-    <col width="9.140625" customWidth="1" style="21" min="8" max="8"/>
-    <col width="10.7109375" customWidth="1" style="21" min="9" max="9"/>
+    <col width="17.85546875" customWidth="1" style="19" min="1" max="1"/>
+    <col width="9.140625" customWidth="1" style="19" min="4" max="4"/>
+    <col width="9.140625" customWidth="1" style="19" min="8" max="8"/>
+    <col width="10.7109375" customWidth="1" style="19" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="18" t="inlineStr">
         <is>
           <t>GERENCIAMENTO DE EQUIPAMENTOS DA TI</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="22" t="inlineStr">
         <is>
           <t>LEGENDA</t>
         </is>
       </c>
-      <c r="H1" s="23" t="n"/>
-      <c r="I1" s="23" t="n"/>
+      <c r="H1" s="17" t="n"/>
+      <c r="I1" s="17" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="20" t="inlineStr">
@@ -682,119 +674,119 @@
           <t>ITENS</t>
         </is>
       </c>
-      <c r="B2" s="24" t="n"/>
-      <c r="C2" s="12" t="inlineStr">
+      <c r="B2" s="21" t="n"/>
+      <c r="C2" s="16" t="inlineStr">
         <is>
           <t>LEGENDA</t>
         </is>
       </c>
-      <c r="D2" s="23" t="n"/>
-      <c r="E2" s="23" t="n"/>
-      <c r="G2" s="2" t="n"/>
-      <c r="H2" s="2" t="n"/>
-      <c r="I2" s="2" t="n"/>
+      <c r="D2" s="17" t="n"/>
+      <c r="E2" s="17" t="n"/>
+      <c r="G2" s="1" t="n"/>
+      <c r="H2" s="1" t="n"/>
+      <c r="I2" s="1" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>TECLADOS</t>
         </is>
       </c>
-      <c r="B3" s="17" t="n">
+      <c r="B3" s="12" t="n">
         <v>15</v>
       </c>
-      <c r="C3" s="16" t="n"/>
-      <c r="D3" s="14" t="n"/>
-      <c r="E3" s="14" t="n"/>
-      <c r="G3" s="9" t="n"/>
-      <c r="H3" s="5" t="inlineStr">
+      <c r="C3" s="11" t="n"/>
+      <c r="D3" s="9" t="n"/>
+      <c r="E3" s="9" t="n"/>
+      <c r="G3" s="6" t="n"/>
+      <c r="H3" s="4" t="inlineStr">
         <is>
           <t>ESTOQUE EM ALTA</t>
         </is>
       </c>
-      <c r="I3" s="2" t="n"/>
+      <c r="I3" s="1" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>MOUSES</t>
         </is>
       </c>
-      <c r="B4" s="18" t="n">
+      <c r="B4" s="13" t="n">
         <v>20</v>
       </c>
-      <c r="C4" s="16" t="n"/>
-      <c r="D4" s="14" t="n"/>
-      <c r="E4" s="14" t="n"/>
-      <c r="G4" s="10" t="n"/>
-      <c r="H4" s="5" t="inlineStr">
+      <c r="C4" s="11" t="n"/>
+      <c r="D4" s="9" t="n"/>
+      <c r="E4" s="9" t="n"/>
+      <c r="G4" s="7" t="n"/>
+      <c r="H4" s="4" t="inlineStr">
         <is>
           <t>ESTOQUE EM QUEDA</t>
         </is>
       </c>
-      <c r="I4" s="5" t="n"/>
+      <c r="I4" s="4" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>H. KJ</t>
         </is>
       </c>
-      <c r="B5" s="18" t="n">
+      <c r="B5" s="13" t="n">
         <v>30</v>
       </c>
-      <c r="C5" s="16" t="n"/>
-      <c r="D5" s="14" t="n"/>
-      <c r="E5" s="14" t="n"/>
-      <c r="G5" s="11" t="n"/>
-      <c r="H5" s="5" t="inlineStr">
+      <c r="C5" s="11" t="n"/>
+      <c r="D5" s="9" t="n"/>
+      <c r="E5" s="9" t="n"/>
+      <c r="G5" s="8" t="n"/>
+      <c r="H5" s="4" t="inlineStr">
         <is>
           <t>SOLICITAR ESTOQUE</t>
         </is>
       </c>
-      <c r="I5" s="2" t="n"/>
+      <c r="I5" s="1" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>H. PnP</t>
         </is>
       </c>
-      <c r="B6" s="18" t="n">
+      <c r="B6" s="13" t="n">
         <v>15</v>
       </c>
-      <c r="C6" s="16" t="n"/>
-      <c r="D6" s="14" t="n"/>
-      <c r="E6" s="14" t="n"/>
-      <c r="G6" s="3" t="n"/>
-      <c r="H6" s="3" t="n"/>
-      <c r="I6" s="3" t="n"/>
+      <c r="C6" s="11" t="n"/>
+      <c r="D6" s="9" t="n"/>
+      <c r="E6" s="9" t="n"/>
+      <c r="G6" s="2" t="n"/>
+      <c r="H6" s="2" t="n"/>
+      <c r="I6" s="2" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="inlineStr">
+      <c r="A7" s="5" t="inlineStr">
         <is>
           <t>CF AMERICANOS</t>
         </is>
       </c>
-      <c r="B7" s="18" t="n">
+      <c r="B7" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="15" t="n"/>
-      <c r="D7" s="14" t="n"/>
-      <c r="E7" s="14" t="n"/>
+      <c r="C7" s="10" t="n"/>
+      <c r="D7" s="9" t="n"/>
+      <c r="E7" s="9" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="inlineStr">
+      <c r="A8" s="3" t="inlineStr">
         <is>
           <t>CF CHINÊS</t>
         </is>
       </c>
-      <c r="B8" s="18" t="n">
+      <c r="B8" s="13" t="n">
         <v>20</v>
       </c>
-      <c r="C8" s="16" t="n"/>
-      <c r="D8" s="14" t="n"/>
-      <c r="E8" s="14" t="n"/>
+      <c r="C8" s="11" t="n"/>
+      <c r="D8" s="9" t="n"/>
+      <c r="E8" s="9" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -813,60 +805,110 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="16" customWidth="1" style="21" min="1" max="1"/>
-    <col width="13.7109375" customWidth="1" style="21" min="2" max="2"/>
-    <col width="18" customWidth="1" style="21" min="3" max="3"/>
-    <col width="17.42578125" bestFit="1" customWidth="1" style="21" min="4" max="4"/>
-    <col width="14.7109375" customWidth="1" style="21" min="5" max="5"/>
+    <col width="16" customWidth="1" style="19" min="1" max="1"/>
+    <col width="19.42578125" customWidth="1" style="19" min="2" max="2"/>
+    <col width="18" customWidth="1" style="19" min="3" max="3"/>
+    <col width="17.42578125" bestFit="1" customWidth="1" style="19" min="4" max="4"/>
+    <col width="14.7109375" customWidth="1" style="19" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="18" t="inlineStr">
         <is>
           <t>REGISTRO DA MOVIMENTAÇÃO DE EQUIPAMENTOS DA TI</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="22" t="inlineStr">
+      <c r="A2" s="14" t="inlineStr">
         <is>
           <t>CHAMADO</t>
         </is>
       </c>
-      <c r="B2" s="22" t="inlineStr">
-        <is>
-          <t>ITEM</t>
-        </is>
-      </c>
-      <c r="C2" s="22" t="inlineStr">
+      <c r="B2" s="14" t="inlineStr">
+        <is>
+          <t>EQUIPAMENTO</t>
+        </is>
+      </c>
+      <c r="C2" s="14" t="inlineStr">
         <is>
           <t>QUANTIDADE</t>
         </is>
       </c>
-      <c r="D2" s="22" t="inlineStr">
+      <c r="D2" s="14" t="inlineStr">
         <is>
           <t>ADIÇÃO OU TROCA</t>
         </is>
       </c>
-      <c r="E2" s="22" t="inlineStr">
+      <c r="E2" s="14" t="inlineStr">
         <is>
           <t>DATA</t>
         </is>
       </c>
     </row>
-    <row r="3"/>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>NULO</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TECLADO</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>SAIDA</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>15/5/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>NULO</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>TECLADO</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="E4" s="15" t="inlineStr">
+        <is>
+          <t>15/5/2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>